<commit_message>
Create test case for login error
</commit_message>
<xml_diff>
--- a/src/main/resources/data_LoginTest.xlsx
+++ b/src/main/resources/data_LoginTest.xlsx
@@ -5,21 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Practices\Excel\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\Practices\AK36\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="valid_Account" sheetId="1" r:id="rId1"/>
+    <sheet name="invalid_Account" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>userName</t>
   </si>
@@ -37,6 +38,33 @@
   </si>
   <si>
     <t>aA@123456</t>
+  </si>
+  <si>
+    <t>Test@1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t>"))@#*@#@_"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">. </t>
+  </si>
+  <si>
+    <t>binhvh3</t>
+  </si>
+  <si>
+    <t>105 OR 1=1</t>
+  </si>
+  <si>
+    <t>" or ""="</t>
   </si>
 </sst>
 </file>
@@ -394,8 +422,8 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,4 +461,83 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>